<commit_message>
updated EPHCC documentation log
</commit_message>
<xml_diff>
--- a/HighLevelDocs/HIL work for improving docs.xlsx
+++ b/HighLevelDocs/HIL work for improving docs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>ActiveLoad</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>Unit test from "CircuitBreaker" should match the "FLS CircuitBreaker"</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R: The folder name can remain the same since it will house the blocks that interface hardware-with-IO cards to the simulation.  However, the names of the libraries for each model should be informative - this block will vary depending on the components interfaced.  </t>
+  </si>
+  <si>
+    <t>R: Do we need unit test for a simple fault?</t>
   </si>
 </sst>
 </file>
@@ -215,17 +224,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -676,7 +732,8 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,474 +742,499 @@
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="81.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="41.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="C21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="3"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:E25">
-    <cfRule type="containsBlanks" dxfId="11" priority="4">
+    <cfRule type="containsBlanks" dxfId="17" priority="4">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:B32">
-    <cfRule type="containsBlanks" dxfId="8" priority="1">
+    <cfRule type="containsBlanks" dxfId="14" priority="1">
       <formula>LEN(TRIM(B29))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>